<commit_message>
Added AGC on/off switch Some minor bug fixes and comments
Signed-off-by: pitschu <peter@pitschu.de>
</commit_message>
<xml_diff>
--- a/Bedienung.xlsx
+++ b/Bedienung.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="28515" windowHeight="12855"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t xml:space="preserve">On/Off </t>
   </si>
@@ -256,13 +256,16 @@
   </si>
   <si>
     <t>Set mode "Fade DIY colors" up to 6 colors in DIY</t>
+  </si>
+  <si>
+    <t>Toggle AGC (auto gain control) on/off</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,11 +366,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -386,6 +389,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -700,7 +708,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -774,6 +782,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -808,6 +817,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -983,17 +993,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="36.85546875" customWidth="1"/>
@@ -1002,21 +1012,21 @@
     <col min="5" max="5" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="5" t="s">
         <v>58</v>
       </c>
@@ -1024,19 +1034,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1048,43 +1058,43 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1098,7 +1108,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1112,7 +1122,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1126,7 +1136,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1138,7 +1148,7 @@
       </c>
       <c r="D12" s="12"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1152,7 +1162,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1166,7 +1176,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1180,7 +1190,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1194,7 +1204,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1208,7 +1218,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1222,31 +1232,31 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1258,7 +1268,7 @@
       </c>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1268,7 +1278,7 @@
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1278,7 +1288,7 @@
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -1288,7 +1298,7 @@
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -1298,7 +1308,7 @@
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -1308,7 +1318,7 @@
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1320,7 +1330,7 @@
       </c>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1330,19 +1340,19 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -1356,37 +1366,32 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="8"/>
+      <c r="D32" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C4:D4"/>
@@ -1397,6 +1402,11 @@
     <mergeCell ref="C21:D26"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId1"/>
@@ -1405,24 +1415,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
V1.2 - fixed bugs in tvp5150:dcmi.c (SLOTs devider) - added dynFramesLimit - some default values updated - avoid black-flickering (ambiLight.c)
Signed-off-by: pitschu <peter@pitschu.de>
</commit_message>
<xml_diff>
--- a/Bedienung.xlsx
+++ b/Bedienung.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="28515" windowHeight="12855"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
   <si>
     <t xml:space="preserve">On/Off </t>
   </si>
@@ -259,13 +259,16 @@
   </si>
   <si>
     <t>Toggle AGC (auto gain control) on/off</t>
+  </si>
+  <si>
+    <t>Quick Reference Guide for pitschu's AmbiLight V1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,7 +307,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -353,11 +356,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -366,11 +378,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -381,6 +393,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -708,7 +723,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -782,7 +797,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -817,7 +831,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -993,17 +1006,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:D32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="36.85546875" customWidth="1"/>
@@ -1012,21 +1025,29 @@
     <col min="5" max="5" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="1" spans="1:4" ht="18.75">
+      <c r="A1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="5" t="s">
         <v>58</v>
       </c>
@@ -1034,19 +1055,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1058,43 +1079,43 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1108,7 +1129,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1122,7 +1143,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1136,7 +1157,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1148,7 +1169,7 @@
       </c>
       <c r="D12" s="12"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1162,7 +1183,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1176,7 +1197,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1190,7 +1211,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1204,7 +1225,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1218,7 +1239,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1232,31 +1253,31 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1268,7 +1289,7 @@
       </c>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1278,7 +1299,7 @@
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1288,7 +1309,7 @@
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -1298,7 +1319,7 @@
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -1308,7 +1329,7 @@
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -1318,7 +1339,7 @@
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1330,7 +1351,7 @@
       </c>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1340,19 +1361,19 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -1366,32 +1387,38 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="6"/>
+      <c r="D32" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C4:D4"/>
@@ -1402,11 +1429,6 @@
     <mergeCell ref="C21:D26"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId1"/>
@@ -1415,24 +1437,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>